<commit_message>
Update script to handle all-caps names, and added a whitelist of common terms to be excluded from redaction.
</commit_message>
<xml_diff>
--- a/PII_Test_File.xlsx
+++ b/PII_Test_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dvagov-my.sharepoint.com/personal/ryan_powers3_va_gov/Documents/Documents/PII Scrubbing Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{95127F26-1053-46A0-9378-8D4C577FAC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D7FCC62-84F5-43DD-86DE-274DFD9151B3}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{95127F26-1053-46A0-9378-8D4C577FAC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E40E751-89EA-4F22-A6EF-60A8CD891F4C}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11265" xr2:uid="{37178256-A5C4-4B55-BE54-168D1F761206}"/>
+    <workbookView xWindow="1635" yWindow="615" windowWidth="26265" windowHeight="13485" xr2:uid="{37178256-A5C4-4B55-BE54-168D1F761206}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,10 +80,10 @@
     <t xml:space="preserve">My social security number is 686549847 can you look up my file. Sarah Rose-Longwell. </t>
   </si>
   <si>
-    <t xml:space="preserve">website could not access my appointments. Mallory Wehan. </t>
+    <t xml:space="preserve">This site is VERY CONFUSING!  My name is Abraham Lincoln! We are not IT tech savvy!  Make it simple for us to send and receive messages from our Medical Providers! JOHN SMITH. </t>
   </si>
   <si>
-    <t xml:space="preserve">This site is VERY CONFUSING!  My name is Abraham Lincoln! We are not IT tech savvy!  Make it simple for us to send and receive messages from our Medical Providers! JOHN SMITH. </t>
+    <t>website could not access my appointments. Mallory Wehan. 978-888-6577</t>
   </si>
 </sst>
 </file>
@@ -523,13 +523,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC298751-4947-4EB7-93D1-1D2C4342191E}">
   <dimension ref="A1:A1917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="1" max="1" width="93.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -587,9 +587,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="30" x14ac:dyDescent="0.25">
@@ -602,9 +602,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30" x14ac:dyDescent="0.25">

</xml_diff>